<commit_message>
Add command to assign players to teams
</commit_message>
<xml_diff>
--- a/SpielerDaten.xlsx
+++ b/SpielerDaten.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>player_firstName</t>
   </si>
@@ -28,6 +28,9 @@
     <t>player_position</t>
   </si>
   <si>
+    <t>player_team</t>
+  </si>
+  <si>
     <t>Franz</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
   </si>
   <si>
     <t>Goalkeeper</t>
+  </si>
+  <si>
+    <t>PPL</t>
   </si>
   <si>
     <t>Michael</t>
@@ -325,13 +331,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>23.0</v>
@@ -340,15 +349,18 @@
         <v>34134.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>57.0</v>
@@ -357,7 +369,10 @@
         <v>31740.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add commands to add locations and link all data
</commit_message>
<xml_diff>
--- a/SpielerDaten.xlsx
+++ b/SpielerDaten.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>player_firstName</t>
   </si>
@@ -50,6 +50,63 @@
   </si>
   <si>
     <t>Sweeper</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Geiger</t>
+  </si>
+  <si>
+    <t>Winger</t>
+  </si>
+  <si>
+    <t>Hells Teddies</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Anninger</t>
+  </si>
+  <si>
+    <t>Attacking Midfielder</t>
+  </si>
+  <si>
+    <t>Elements</t>
+  </si>
+  <si>
+    <t>Phillipp</t>
+  </si>
+  <si>
+    <t>Stöllinger</t>
+  </si>
+  <si>
+    <t>Central Midfielder</t>
+  </si>
+  <si>
+    <t>Valantic</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Meier</t>
+  </si>
+  <si>
+    <t>Center Back</t>
+  </si>
+  <si>
+    <t>New Team</t>
+  </si>
+  <si>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>Forsthuber</t>
+  </si>
+  <si>
+    <t>Alchimiste</t>
   </si>
 </sst>
 </file>
@@ -59,10 +116,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -86,14 +149,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -313,6 +380,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="14.38"/>
+    <col customWidth="1" min="5" max="5" width="15.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -334,45 +402,165 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>23.0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>34134.0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>57.0</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>31740.0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>34846.0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>34532.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>33786.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>34034.0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>33544.0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>